<commit_message>
fix: clarified value[x] in components
</commit_message>
<xml_diff>
--- a/Mappings/ComfortScale - STU3.xlsx
+++ b/Mappings/ComfortScale - STU3.xlsx
@@ -871,9 +871,6 @@
     <t>.valueQuantity</t>
   </si>
   <si>
-    <t>.component.slice</t>
-  </si>
-  <si>
     <t>.effectiveDateTime</t>
   </si>
   <si>
@@ -929,6 +926,9 @@
   </si>
   <si>
     <t xml:space="preserve">Google </t>
+  </si>
+  <si>
+    <t>.component.slice.valueCodeableConcept</t>
   </si>
 </sst>
 </file>
@@ -2442,57 +2442,57 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B1" t="s">
         <v>285</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>286</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>287</v>
-      </c>
-      <c r="F1" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C3" s="20" t="s">
         <v>71</v>
       </c>
       <c r="F3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C8" s="20" t="s">
         <v>71</v>
@@ -2500,24 +2500,24 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C9" s="20" t="s">
         <v>71</v>
       </c>
       <c r="F9" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C10" s="20" t="s">
         <v>71</v>
       </c>
       <c r="F10" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -2530,7 +2530,7 @@
   <dimension ref="B2:S13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2584,10 +2584,10 @@
         <v>276</v>
       </c>
       <c r="Q2" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="R2" s="17" t="s">
         <v>283</v>
-      </c>
-      <c r="R2" s="17" t="s">
-        <v>284</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>70</v>
@@ -2622,7 +2622,7 @@
         <v>277</v>
       </c>
       <c r="Q3" s="18" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
@@ -2660,14 +2660,14 @@
         <v>278</v>
       </c>
       <c r="Q4" s="19" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R4" s="2"/>
       <c r="S4" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="2:19">
+    <row r="5" spans="2:19" ht="25.5">
       <c r="B5" s="11"/>
       <c r="C5" s="12" t="s">
         <v>84</v>
@@ -2699,15 +2699,15 @@
         <v>89</v>
       </c>
       <c r="P5" s="16" t="s">
-        <v>279</v>
+        <v>298</v>
       </c>
       <c r="Q5" s="19" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R5" s="16"/>
       <c r="S5" s="2"/>
     </row>
-    <row r="6" spans="2:19">
+    <row r="6" spans="2:19" ht="25.5">
       <c r="B6" s="11"/>
       <c r="C6" s="12" t="s">
         <v>90</v>
@@ -2739,15 +2739,15 @@
         <v>94</v>
       </c>
       <c r="P6" s="16" t="s">
-        <v>279</v>
+        <v>298</v>
       </c>
       <c r="Q6" s="19" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R6" s="16"/>
       <c r="S6" s="2"/>
     </row>
-    <row r="7" spans="2:19">
+    <row r="7" spans="2:19" ht="25.5">
       <c r="B7" s="11"/>
       <c r="C7" s="12" t="s">
         <v>95</v>
@@ -2779,15 +2779,15 @@
         <v>99</v>
       </c>
       <c r="P7" s="16" t="s">
-        <v>279</v>
+        <v>298</v>
       </c>
       <c r="Q7" s="19" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R7" s="16"/>
       <c r="S7" s="2"/>
     </row>
-    <row r="8" spans="2:19">
+    <row r="8" spans="2:19" ht="25.5">
       <c r="B8" s="11"/>
       <c r="C8" s="12" t="s">
         <v>100</v>
@@ -2819,15 +2819,15 @@
         <v>104</v>
       </c>
       <c r="P8" s="16" t="s">
-        <v>279</v>
+        <v>298</v>
       </c>
       <c r="Q8" s="19" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R8" s="16"/>
       <c r="S8" s="2"/>
     </row>
-    <row r="9" spans="2:19">
+    <row r="9" spans="2:19" ht="25.5">
       <c r="B9" s="11"/>
       <c r="C9" s="12" t="s">
         <v>105</v>
@@ -2859,15 +2859,15 @@
         <v>109</v>
       </c>
       <c r="P9" s="16" t="s">
-        <v>279</v>
+        <v>298</v>
       </c>
       <c r="Q9" s="19" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R9" s="16"/>
       <c r="S9" s="2"/>
     </row>
-    <row r="10" spans="2:19">
+    <row r="10" spans="2:19" ht="25.5">
       <c r="B10" s="11"/>
       <c r="C10" s="12" t="s">
         <v>110</v>
@@ -2899,15 +2899,15 @@
         <v>114</v>
       </c>
       <c r="P10" s="16" t="s">
-        <v>279</v>
+        <v>298</v>
       </c>
       <c r="Q10" s="19" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R10" s="16"/>
       <c r="S10" s="2"/>
     </row>
-    <row r="11" spans="2:19">
+    <row r="11" spans="2:19" ht="25.5">
       <c r="B11" s="11"/>
       <c r="C11" s="12" t="s">
         <v>115</v>
@@ -2939,10 +2939,10 @@
         <v>119</v>
       </c>
       <c r="P11" s="16" t="s">
-        <v>279</v>
+        <v>298</v>
       </c>
       <c r="Q11" s="19" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R11" s="16"/>
       <c r="S11" s="2"/>
@@ -2977,7 +2977,7 @@
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
       <c r="P12" s="16" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="Q12" s="16"/>
       <c r="R12" s="16"/>
@@ -3015,7 +3015,7 @@
       </c>
       <c r="O13" s="2"/>
       <c r="P13" s="16" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Q13" s="16"/>
       <c r="R13" s="16"/>

</xml_diff>